<commit_message>
Use POm in project
</commit_message>
<xml_diff>
--- a/vtiger-crm-a12/src/test/resources/testScriptData.xlsx
+++ b/vtiger-crm-a12/src/test/resources/testScriptData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit Sharma\Desktop\Selenium\vtiger-crm-a12\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit Sharma\git\Vtiger-crm-fw\vtiger-crm-a12\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385FD4C4-EB91-46E9-93C7-614BD072AF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88666E5-5CB8-4B25-A749-46188FE2B2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FavCar" sheetId="1" r:id="rId1"/>
     <sheet name="FavBike" sheetId="2" r:id="rId2"/>
     <sheet name="Contact" sheetId="3" r:id="rId3"/>
     <sheet name="Class1" sheetId="4" r:id="rId4"/>
-    <sheet name="Class2" sheetId="5" r:id="rId5"/>
+    <sheet name="Organization" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>CarName</t>
   </si>
@@ -212,6 +212,39 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>TCS</t>
+  </si>
+  <si>
+    <t>TATA</t>
+  </si>
+  <si>
+    <t>WIPRO</t>
+  </si>
+  <si>
+    <t>META</t>
+  </si>
+  <si>
+    <t>HCL</t>
+  </si>
+  <si>
+    <t>AMUL</t>
+  </si>
+  <si>
+    <t>MRF</t>
+  </si>
+  <si>
+    <t>HONDA</t>
+  </si>
+  <si>
+    <t>TOYOTA</t>
+  </si>
+  <si>
+    <t>GOOGLE</t>
   </si>
 </sst>
 </file>
@@ -409,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -429,6 +462,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1002,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5A7FAC-7878-486A-B10A-0C5E52393DAC}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1152,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0B53DD-9CDB-4BEA-8CF6-8A98AC42E82D}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,84 +1200,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="11">
-        <v>1</v>
+      <c r="A1" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
-        <v>2</v>
+      <c r="A2" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
-        <v>3</v>
+      <c r="A3" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="A4" s="11" t="s">
+        <v>64</v>
+      </c>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
+      <c r="A5" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+      <c r="A6" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
+      <c r="A7" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+      <c r="A8" s="15" t="s">
+        <v>68</v>
+      </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+      <c r="A9" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+      <c r="A10" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="B10" s="10"/>
       <c r="C10" s="14"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+      <c r="A11" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="15" t="s">
+        <v>69</v>
+      </c>
       <c r="B12" s="10"/>
       <c r="C12" s="14"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="15" t="s">
+        <v>70</v>
+      </c>
       <c r="B13" s="10"/>
       <c r="C13" s="14"/>
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
+      <c r="A14" s="15" t="s">
+        <v>71</v>
+      </c>
       <c r="B14" s="10"/>
       <c r="C14" s="14"/>
     </row>

</xml_diff>